<commit_message>
Création extension lieu dit 022f7723ca6844f2a79c7ba0204d9023a4629e85
</commit_message>
<xml_diff>
--- a/ig/291-erreur-organization-lieu-dit-precinct/StructureDefinition-ror-location.xlsx
+++ b/ig/291-erreur-organization-lieu-dit-precinct/StructureDefinition-ror-location.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4641" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4641" uniqueCount="729">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-05T13:07:25+00:00</t>
+    <t>2024-02-05T13:19:57+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1849,25 +1849,6 @@
     <t>ADXP[partType=STB]</t>
   </si>
   <si>
-    <t>Location.address.line.extension:precinct</t>
-  </si>
-  <si>
-    <t>precinct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {iso21090-ADXP-precinct}
-</t>
-  </si>
-  <si>
-    <t>lieuDit (Adresse) : Lieu qui porte un nom rappelant une particularité topographique ou historique</t>
-  </si>
-  <si>
-    <t>A subsection of a municipality.</t>
-  </si>
-  <si>
-    <t>ADXP[partType=PRE]</t>
-  </si>
-  <si>
     <t>Location.address.line.extension:postalBox</t>
   </si>
   <si>
@@ -1885,6 +1866,22 @@
   </si>
   <si>
     <t>ADXP[partType=POB]</t>
+  </si>
+  <si>
+    <t>Location.address.line.extension:lieuDit</t>
+  </si>
+  <si>
+    <t>lieuDit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/ror/StructureDefinition/ror-lieu-dit}
+</t>
+  </si>
+  <si>
+    <t>lieuDit (Adresse) : Lieu qui porte un nom rappelant une particularité topographique ou historique</t>
+  </si>
+  <si>
+    <t>Extension créée dans le cadre du ROR pour indiquer le lieu dit</t>
   </si>
   <si>
     <t>Location.address.line.value</t>
@@ -14222,7 +14219,7 @@
         <v>114</v>
       </c>
       <c r="AK107" t="s" s="2">
-        <v>603</v>
+        <v>74</v>
       </c>
       <c r="AL107" t="s" s="2">
         <v>74</v>
@@ -14230,10 +14227,10 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B108" t="s" s="2">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" t="s" s="2">
@@ -14259,10 +14256,10 @@
         <v>99</v>
       </c>
       <c r="L108" t="s" s="2">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="M108" t="s" s="2">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="N108" s="2"/>
       <c r="O108" s="2"/>
@@ -14286,34 +14283,34 @@
         <v>74</v>
       </c>
       <c r="W108" t="s" s="2">
+        <v>605</v>
+      </c>
+      <c r="X108" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y108" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z108" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA108" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB108" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC108" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD108" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE108" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF108" t="s" s="2">
         <v>606</v>
-      </c>
-      <c r="X108" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Y108" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Z108" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AA108" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AB108" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC108" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD108" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE108" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AF108" t="s" s="2">
-        <v>607</v>
       </c>
       <c r="AG108" t="s" s="2">
         <v>75</v>
@@ -14336,14 +14333,14 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B109" t="s" s="2">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" t="s" s="2">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109" t="s" s="2">
@@ -14365,10 +14362,10 @@
         <v>99</v>
       </c>
       <c r="L109" t="s" s="2">
+        <v>609</v>
+      </c>
+      <c r="M109" t="s" s="2">
         <v>610</v>
-      </c>
-      <c r="M109" t="s" s="2">
-        <v>611</v>
       </c>
       <c r="N109" t="s" s="2">
         <v>300</v>
@@ -14385,43 +14382,43 @@
         <v>74</v>
       </c>
       <c r="T109" t="s" s="2">
+        <v>611</v>
+      </c>
+      <c r="U109" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V109" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W109" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X109" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y109" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z109" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA109" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB109" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC109" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD109" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE109" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF109" t="s" s="2">
         <v>612</v>
-      </c>
-      <c r="U109" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="V109" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="W109" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="X109" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Y109" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Z109" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AA109" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AB109" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC109" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD109" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE109" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AF109" t="s" s="2">
-        <v>613</v>
       </c>
       <c r="AG109" t="s" s="2">
         <v>75</v>
@@ -14436,7 +14433,7 @@
         <v>96</v>
       </c>
       <c r="AK109" t="s" s="2">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="AL109" t="s" s="2">
         <v>74</v>
@@ -14444,14 +14441,14 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B110" t="s" s="2">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" t="s" s="2">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E110" s="2"/>
       <c r="F110" t="s" s="2">
@@ -14473,13 +14470,13 @@
         <v>99</v>
       </c>
       <c r="L110" t="s" s="2">
+        <v>616</v>
+      </c>
+      <c r="M110" t="s" s="2">
         <v>617</v>
       </c>
-      <c r="M110" t="s" s="2">
+      <c r="N110" t="s" s="2">
         <v>618</v>
-      </c>
-      <c r="N110" t="s" s="2">
-        <v>619</v>
       </c>
       <c r="O110" s="2"/>
       <c r="P110" t="s" s="2">
@@ -14493,43 +14490,43 @@
         <v>74</v>
       </c>
       <c r="T110" t="s" s="2">
+        <v>619</v>
+      </c>
+      <c r="U110" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V110" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W110" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X110" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y110" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z110" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA110" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB110" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC110" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD110" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE110" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF110" t="s" s="2">
         <v>620</v>
-      </c>
-      <c r="U110" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="V110" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="W110" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="X110" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Y110" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Z110" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AA110" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AB110" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC110" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD110" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE110" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AF110" t="s" s="2">
-        <v>621</v>
       </c>
       <c r="AG110" t="s" s="2">
         <v>75</v>
@@ -14544,7 +14541,7 @@
         <v>96</v>
       </c>
       <c r="AK110" t="s" s="2">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="AL110" t="s" s="2">
         <v>74</v>
@@ -14552,14 +14549,14 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B111" t="s" s="2">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" t="s" s="2">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111" t="s" s="2">
@@ -14581,10 +14578,10 @@
         <v>99</v>
       </c>
       <c r="L111" t="s" s="2">
+        <v>624</v>
+      </c>
+      <c r="M111" t="s" s="2">
         <v>625</v>
-      </c>
-      <c r="M111" t="s" s="2">
-        <v>626</v>
       </c>
       <c r="N111" t="s" s="2">
         <v>300</v>
@@ -14637,7 +14634,7 @@
         <v>74</v>
       </c>
       <c r="AF111" t="s" s="2">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="AG111" t="s" s="2">
         <v>75</v>
@@ -14652,7 +14649,7 @@
         <v>96</v>
       </c>
       <c r="AK111" t="s" s="2">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="AL111" t="s" s="2">
         <v>74</v>
@@ -14660,14 +14657,14 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B112" t="s" s="2">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" t="s" s="2">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112" t="s" s="2">
@@ -14689,10 +14686,10 @@
         <v>99</v>
       </c>
       <c r="L112" t="s" s="2">
+        <v>630</v>
+      </c>
+      <c r="M112" t="s" s="2">
         <v>631</v>
-      </c>
-      <c r="M112" t="s" s="2">
-        <v>632</v>
       </c>
       <c r="N112" t="s" s="2">
         <v>300</v>
@@ -14709,43 +14706,43 @@
         <v>74</v>
       </c>
       <c r="T112" t="s" s="2">
+        <v>632</v>
+      </c>
+      <c r="U112" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V112" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W112" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X112" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y112" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z112" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA112" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB112" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC112" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD112" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE112" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF112" t="s" s="2">
         <v>633</v>
-      </c>
-      <c r="U112" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="V112" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="W112" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="X112" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Y112" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Z112" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AA112" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AB112" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC112" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD112" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE112" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AF112" t="s" s="2">
-        <v>634</v>
       </c>
       <c r="AG112" t="s" s="2">
         <v>75</v>
@@ -14760,7 +14757,7 @@
         <v>96</v>
       </c>
       <c r="AK112" t="s" s="2">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="AL112" t="s" s="2">
         <v>74</v>
@@ -14768,10 +14765,10 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B113" t="s" s="2">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" t="s" s="2">
@@ -14797,13 +14794,13 @@
         <v>99</v>
       </c>
       <c r="L113" t="s" s="2">
+        <v>636</v>
+      </c>
+      <c r="M113" t="s" s="2">
         <v>637</v>
       </c>
-      <c r="M113" t="s" s="2">
+      <c r="N113" t="s" s="2">
         <v>638</v>
-      </c>
-      <c r="N113" t="s" s="2">
-        <v>639</v>
       </c>
       <c r="O113" s="2"/>
       <c r="P113" t="s" s="2">
@@ -14853,7 +14850,7 @@
         <v>74</v>
       </c>
       <c r="AF113" t="s" s="2">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="AG113" t="s" s="2">
         <v>75</v>
@@ -14868,7 +14865,7 @@
         <v>96</v>
       </c>
       <c r="AK113" t="s" s="2">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="AL113" t="s" s="2">
         <v>74</v>
@@ -14876,10 +14873,10 @@
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B114" t="s" s="2">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" t="s" s="2">
@@ -14905,16 +14902,16 @@
         <v>348</v>
       </c>
       <c r="L114" t="s" s="2">
+        <v>642</v>
+      </c>
+      <c r="M114" t="s" s="2">
         <v>643</v>
-      </c>
-      <c r="M114" t="s" s="2">
-        <v>644</v>
       </c>
       <c r="N114" t="s" s="2">
         <v>351</v>
       </c>
       <c r="O114" t="s" s="2">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="P114" t="s" s="2">
         <v>74</v>
@@ -14927,43 +14924,43 @@
         <v>74</v>
       </c>
       <c r="T114" t="s" s="2">
+        <v>645</v>
+      </c>
+      <c r="U114" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V114" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W114" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X114" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y114" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z114" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA114" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB114" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC114" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD114" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE114" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF114" t="s" s="2">
         <v>646</v>
-      </c>
-      <c r="U114" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="V114" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="W114" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="X114" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Y114" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Z114" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AA114" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AB114" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC114" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD114" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE114" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AF114" t="s" s="2">
-        <v>647</v>
       </c>
       <c r="AG114" t="s" s="2">
         <v>75</v>
@@ -14986,10 +14983,10 @@
     </row>
     <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B115" t="s" s="2">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" t="s" s="2">
@@ -15015,16 +15012,16 @@
         <v>257</v>
       </c>
       <c r="L115" t="s" s="2">
+        <v>648</v>
+      </c>
+      <c r="M115" t="s" s="2">
         <v>649</v>
-      </c>
-      <c r="M115" t="s" s="2">
-        <v>650</v>
       </c>
       <c r="N115" t="s" s="2">
         <v>429</v>
       </c>
       <c r="O115" t="s" s="2">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="P115" t="s" s="2">
         <v>74</v>
@@ -15052,11 +15049,11 @@
         <v>152</v>
       </c>
       <c r="Y115" t="s" s="2">
+        <v>651</v>
+      </c>
+      <c r="Z115" t="s" s="2">
         <v>652</v>
       </c>
-      <c r="Z115" t="s" s="2">
-        <v>653</v>
-      </c>
       <c r="AA115" t="s" s="2">
         <v>74</v>
       </c>
@@ -15073,7 +15070,7 @@
         <v>74</v>
       </c>
       <c r="AF115" t="s" s="2">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AG115" t="s" s="2">
         <v>75</v>
@@ -15088,7 +15085,7 @@
         <v>96</v>
       </c>
       <c r="AK115" t="s" s="2">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="AL115" t="s" s="2">
         <v>425</v>
@@ -15096,10 +15093,10 @@
     </row>
     <row r="116" hidden="true">
       <c r="A116" t="s" s="2">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B116" t="s" s="2">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" t="s" s="2">
@@ -15122,17 +15119,17 @@
         <v>74</v>
       </c>
       <c r="K116" t="s" s="2">
+        <v>655</v>
+      </c>
+      <c r="L116" t="s" s="2">
         <v>656</v>
       </c>
-      <c r="L116" t="s" s="2">
+      <c r="M116" t="s" s="2">
         <v>657</v>
-      </c>
-      <c r="M116" t="s" s="2">
-        <v>658</v>
       </c>
       <c r="N116" s="2"/>
       <c r="O116" t="s" s="2">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="P116" t="s" s="2">
         <v>74</v>
@@ -15181,7 +15178,7 @@
         <v>74</v>
       </c>
       <c r="AF116" t="s" s="2">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="AG116" t="s" s="2">
         <v>75</v>
@@ -15196,7 +15193,7 @@
         <v>96</v>
       </c>
       <c r="AK116" t="s" s="2">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="AL116" t="s" s="2">
         <v>74</v>
@@ -15204,10 +15201,10 @@
     </row>
     <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B117" t="s" s="2">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" t="s" s="2">
@@ -15310,10 +15307,10 @@
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B118" t="s" s="2">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" t="s" s="2">
@@ -15418,13 +15415,13 @@
     </row>
     <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
+        <v>662</v>
+      </c>
+      <c r="B119" t="s" s="2">
+        <v>661</v>
+      </c>
+      <c r="C119" t="s" s="2">
         <v>663</v>
-      </c>
-      <c r="B119" t="s" s="2">
-        <v>662</v>
-      </c>
-      <c r="C119" t="s" s="2">
-        <v>664</v>
       </c>
       <c r="D119" t="s" s="2">
         <v>74</v>
@@ -15446,13 +15443,13 @@
         <v>74</v>
       </c>
       <c r="K119" t="s" s="2">
+        <v>664</v>
+      </c>
+      <c r="L119" t="s" s="2">
         <v>665</v>
       </c>
-      <c r="L119" t="s" s="2">
+      <c r="M119" t="s" s="2">
         <v>666</v>
-      </c>
-      <c r="M119" t="s" s="2">
-        <v>667</v>
       </c>
       <c r="N119" s="2"/>
       <c r="O119" s="2"/>
@@ -15526,14 +15523,14 @@
     </row>
     <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B120" t="s" s="2">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" t="s" s="2">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120" t="s" s="2">
@@ -15555,10 +15552,10 @@
         <v>106</v>
       </c>
       <c r="L120" t="s" s="2">
+        <v>669</v>
+      </c>
+      <c r="M120" t="s" s="2">
         <v>670</v>
-      </c>
-      <c r="M120" t="s" s="2">
-        <v>671</v>
       </c>
       <c r="N120" t="s" s="2">
         <v>109</v>
@@ -15613,7 +15610,7 @@
         <v>74</v>
       </c>
       <c r="AF120" t="s" s="2">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="AG120" t="s" s="2">
         <v>75</v>
@@ -15636,10 +15633,10 @@
     </row>
     <row r="121" hidden="true">
       <c r="A121" t="s" s="2">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B121" t="s" s="2">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" t="s" s="2">
@@ -15662,16 +15659,16 @@
         <v>74</v>
       </c>
       <c r="K121" t="s" s="2">
+        <v>673</v>
+      </c>
+      <c r="L121" t="s" s="2">
         <v>674</v>
       </c>
-      <c r="L121" t="s" s="2">
+      <c r="M121" t="s" s="2">
         <v>675</v>
       </c>
-      <c r="M121" t="s" s="2">
+      <c r="N121" t="s" s="2">
         <v>676</v>
-      </c>
-      <c r="N121" t="s" s="2">
-        <v>677</v>
       </c>
       <c r="O121" s="2"/>
       <c r="P121" t="s" s="2">
@@ -15721,7 +15718,7 @@
         <v>74</v>
       </c>
       <c r="AF121" t="s" s="2">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="AG121" t="s" s="2">
         <v>83</v>
@@ -15736,7 +15733,7 @@
         <v>96</v>
       </c>
       <c r="AK121" t="s" s="2">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="AL121" t="s" s="2">
         <v>74</v>
@@ -15744,10 +15741,10 @@
     </row>
     <row r="122" hidden="true">
       <c r="A122" t="s" s="2">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B122" t="s" s="2">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" t="s" s="2">
@@ -15770,16 +15767,16 @@
         <v>74</v>
       </c>
       <c r="K122" t="s" s="2">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="L122" t="s" s="2">
+        <v>679</v>
+      </c>
+      <c r="M122" t="s" s="2">
         <v>680</v>
       </c>
-      <c r="M122" t="s" s="2">
-        <v>681</v>
-      </c>
       <c r="N122" t="s" s="2">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="O122" s="2"/>
       <c r="P122" t="s" s="2">
@@ -15829,7 +15826,7 @@
         <v>74</v>
       </c>
       <c r="AF122" t="s" s="2">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="AG122" t="s" s="2">
         <v>83</v>
@@ -15844,7 +15841,7 @@
         <v>96</v>
       </c>
       <c r="AK122" t="s" s="2">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="AL122" t="s" s="2">
         <v>74</v>
@@ -15852,10 +15849,10 @@
     </row>
     <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B123" t="s" s="2">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" t="s" s="2">
@@ -15878,16 +15875,16 @@
         <v>74</v>
       </c>
       <c r="K123" t="s" s="2">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="L123" t="s" s="2">
+        <v>682</v>
+      </c>
+      <c r="M123" t="s" s="2">
         <v>683</v>
       </c>
-      <c r="M123" t="s" s="2">
-        <v>684</v>
-      </c>
       <c r="N123" t="s" s="2">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="O123" s="2"/>
       <c r="P123" t="s" s="2">
@@ -15937,7 +15934,7 @@
         <v>74</v>
       </c>
       <c r="AF123" t="s" s="2">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="AG123" t="s" s="2">
         <v>75</v>
@@ -15952,7 +15949,7 @@
         <v>96</v>
       </c>
       <c r="AK123" t="s" s="2">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="AL123" t="s" s="2">
         <v>74</v>
@@ -15960,10 +15957,10 @@
     </row>
     <row r="124" hidden="true">
       <c r="A124" t="s" s="2">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B124" t="s" s="2">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C124" s="2"/>
       <c r="D124" t="s" s="2">
@@ -15989,16 +15986,16 @@
         <v>357</v>
       </c>
       <c r="L124" t="s" s="2">
+        <v>685</v>
+      </c>
+      <c r="M124" t="s" s="2">
         <v>686</v>
       </c>
-      <c r="M124" t="s" s="2">
+      <c r="N124" t="s" s="2">
         <v>687</v>
       </c>
-      <c r="N124" t="s" s="2">
+      <c r="O124" t="s" s="2">
         <v>688</v>
-      </c>
-      <c r="O124" t="s" s="2">
-        <v>689</v>
       </c>
       <c r="P124" t="s" s="2">
         <v>74</v>
@@ -16047,7 +16044,7 @@
         <v>74</v>
       </c>
       <c r="AF124" t="s" s="2">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AG124" t="s" s="2">
         <v>75</v>
@@ -16062,7 +16059,7 @@
         <v>362</v>
       </c>
       <c r="AK124" t="s" s="2">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="AL124" t="s" s="2">
         <v>74</v>
@@ -16070,10 +16067,10 @@
     </row>
     <row r="125" hidden="true">
       <c r="A125" t="s" s="2">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B125" t="s" s="2">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C125" s="2"/>
       <c r="D125" t="s" s="2">
@@ -16096,19 +16093,19 @@
         <v>74</v>
       </c>
       <c r="K125" t="s" s="2">
+        <v>691</v>
+      </c>
+      <c r="L125" t="s" s="2">
         <v>692</v>
       </c>
-      <c r="L125" t="s" s="2">
+      <c r="M125" t="s" s="2">
         <v>693</v>
       </c>
-      <c r="M125" t="s" s="2">
+      <c r="N125" t="s" s="2">
         <v>694</v>
       </c>
-      <c r="N125" t="s" s="2">
+      <c r="O125" t="s" s="2">
         <v>695</v>
-      </c>
-      <c r="O125" t="s" s="2">
-        <v>696</v>
       </c>
       <c r="P125" t="s" s="2">
         <v>74</v>
@@ -16157,7 +16154,7 @@
         <v>74</v>
       </c>
       <c r="AF125" t="s" s="2">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="AG125" t="s" s="2">
         <v>75</v>
@@ -16172,7 +16169,7 @@
         <v>362</v>
       </c>
       <c r="AK125" t="s" s="2">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="AL125" t="s" s="2">
         <v>74</v>
@@ -16180,10 +16177,10 @@
     </row>
     <row r="126" hidden="true">
       <c r="A126" t="s" s="2">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B126" t="s" s="2">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" t="s" s="2">
@@ -16206,16 +16203,16 @@
         <v>74</v>
       </c>
       <c r="K126" t="s" s="2">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="L126" t="s" s="2">
+        <v>698</v>
+      </c>
+      <c r="M126" t="s" s="2">
         <v>699</v>
       </c>
-      <c r="M126" t="s" s="2">
+      <c r="N126" t="s" s="2">
         <v>700</v>
-      </c>
-      <c r="N126" t="s" s="2">
-        <v>701</v>
       </c>
       <c r="O126" s="2"/>
       <c r="P126" t="s" s="2">
@@ -16265,7 +16262,7 @@
         <v>74</v>
       </c>
       <c r="AF126" t="s" s="2">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="AG126" t="s" s="2">
         <v>75</v>
@@ -16280,7 +16277,7 @@
         <v>96</v>
       </c>
       <c r="AK126" t="s" s="2">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="AL126" t="s" s="2">
         <v>74</v>
@@ -16288,10 +16285,10 @@
     </row>
     <row r="127" hidden="true">
       <c r="A127" t="s" s="2">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B127" t="s" s="2">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C127" s="2"/>
       <c r="D127" t="s" s="2">
@@ -16394,10 +16391,10 @@
     </row>
     <row r="128" hidden="true">
       <c r="A128" t="s" s="2">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B128" t="s" s="2">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C128" s="2"/>
       <c r="D128" t="s" s="2">
@@ -16502,14 +16499,14 @@
     </row>
     <row r="129" hidden="true">
       <c r="A129" t="s" s="2">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B129" t="s" s="2">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C129" s="2"/>
       <c r="D129" t="s" s="2">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E129" s="2"/>
       <c r="F129" t="s" s="2">
@@ -16531,10 +16528,10 @@
         <v>106</v>
       </c>
       <c r="L129" t="s" s="2">
+        <v>669</v>
+      </c>
+      <c r="M129" t="s" s="2">
         <v>670</v>
-      </c>
-      <c r="M129" t="s" s="2">
-        <v>671</v>
       </c>
       <c r="N129" t="s" s="2">
         <v>109</v>
@@ -16589,7 +16586,7 @@
         <v>74</v>
       </c>
       <c r="AF129" t="s" s="2">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="AG129" t="s" s="2">
         <v>75</v>
@@ -16612,10 +16609,10 @@
     </row>
     <row r="130" hidden="true">
       <c r="A130" t="s" s="2">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B130" t="s" s="2">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C130" s="2"/>
       <c r="D130" t="s" s="2">
@@ -16641,10 +16638,10 @@
         <v>167</v>
       </c>
       <c r="L130" t="s" s="2">
+        <v>706</v>
+      </c>
+      <c r="M130" t="s" s="2">
         <v>707</v>
-      </c>
-      <c r="M130" t="s" s="2">
-        <v>708</v>
       </c>
       <c r="N130" t="s" s="2">
         <v>300</v>
@@ -16676,11 +16673,11 @@
         <v>159</v>
       </c>
       <c r="Y130" t="s" s="2">
+        <v>708</v>
+      </c>
+      <c r="Z130" t="s" s="2">
         <v>709</v>
       </c>
-      <c r="Z130" t="s" s="2">
-        <v>710</v>
-      </c>
       <c r="AA130" t="s" s="2">
         <v>74</v>
       </c>
@@ -16697,7 +16694,7 @@
         <v>74</v>
       </c>
       <c r="AF130" t="s" s="2">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="AG130" t="s" s="2">
         <v>75</v>
@@ -16712,7 +16709,7 @@
         <v>96</v>
       </c>
       <c r="AK130" t="s" s="2">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="AL130" t="s" s="2">
         <v>74</v>
@@ -16720,10 +16717,10 @@
     </row>
     <row r="131" hidden="true">
       <c r="A131" t="s" s="2">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B131" t="s" s="2">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C131" s="2"/>
       <c r="D131" t="s" s="2">
@@ -16749,10 +16746,10 @@
         <v>314</v>
       </c>
       <c r="L131" t="s" s="2">
+        <v>711</v>
+      </c>
+      <c r="M131" t="s" s="2">
         <v>712</v>
-      </c>
-      <c r="M131" t="s" s="2">
-        <v>713</v>
       </c>
       <c r="N131" s="2"/>
       <c r="O131" s="2"/>
@@ -16803,7 +16800,7 @@
         <v>74</v>
       </c>
       <c r="AF131" t="s" s="2">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="AG131" t="s" s="2">
         <v>75</v>
@@ -16818,7 +16815,7 @@
         <v>96</v>
       </c>
       <c r="AK131" t="s" s="2">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="AL131" t="s" s="2">
         <v>74</v>
@@ -16826,10 +16823,10 @@
     </row>
     <row r="132" hidden="true">
       <c r="A132" t="s" s="2">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B132" t="s" s="2">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C132" s="2"/>
       <c r="D132" t="s" s="2">
@@ -16852,13 +16849,13 @@
         <v>74</v>
       </c>
       <c r="K132" t="s" s="2">
+        <v>714</v>
+      </c>
+      <c r="L132" t="s" s="2">
         <v>715</v>
       </c>
-      <c r="L132" t="s" s="2">
+      <c r="M132" t="s" s="2">
         <v>716</v>
-      </c>
-      <c r="M132" t="s" s="2">
-        <v>717</v>
       </c>
       <c r="N132" s="2"/>
       <c r="O132" s="2"/>
@@ -16909,7 +16906,7 @@
         <v>74</v>
       </c>
       <c r="AF132" t="s" s="2">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="AG132" t="s" s="2">
         <v>75</v>
@@ -16924,7 +16921,7 @@
         <v>96</v>
       </c>
       <c r="AK132" t="s" s="2">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="AL132" t="s" s="2">
         <v>74</v>
@@ -16932,10 +16929,10 @@
     </row>
     <row r="133" hidden="true">
       <c r="A133" t="s" s="2">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B133" t="s" s="2">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C133" s="2"/>
       <c r="D133" t="s" s="2">
@@ -16958,13 +16955,13 @@
         <v>74</v>
       </c>
       <c r="K133" t="s" s="2">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="L133" t="s" s="2">
+        <v>718</v>
+      </c>
+      <c r="M133" t="s" s="2">
         <v>719</v>
-      </c>
-      <c r="M133" t="s" s="2">
-        <v>720</v>
       </c>
       <c r="N133" s="2"/>
       <c r="O133" s="2"/>
@@ -17015,7 +17012,7 @@
         <v>74</v>
       </c>
       <c r="AF133" t="s" s="2">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="AG133" t="s" s="2">
         <v>75</v>
@@ -17030,7 +17027,7 @@
         <v>96</v>
       </c>
       <c r="AK133" t="s" s="2">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="AL133" t="s" s="2">
         <v>74</v>
@@ -17038,10 +17035,10 @@
     </row>
     <row r="134" hidden="true">
       <c r="A134" t="s" s="2">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B134" t="s" s="2">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C134" s="2"/>
       <c r="D134" t="s" s="2">
@@ -17067,10 +17064,10 @@
         <v>99</v>
       </c>
       <c r="L134" t="s" s="2">
+        <v>721</v>
+      </c>
+      <c r="M134" t="s" s="2">
         <v>722</v>
-      </c>
-      <c r="M134" t="s" s="2">
-        <v>723</v>
       </c>
       <c r="N134" t="s" s="2">
         <v>300</v>
@@ -17123,7 +17120,7 @@
         <v>74</v>
       </c>
       <c r="AF134" t="s" s="2">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="AG134" t="s" s="2">
         <v>75</v>
@@ -17146,10 +17143,10 @@
     </row>
     <row r="135" hidden="true">
       <c r="A135" t="s" s="2">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B135" t="s" s="2">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C135" s="2"/>
       <c r="D135" t="s" s="2">
@@ -17172,19 +17169,19 @@
         <v>74</v>
       </c>
       <c r="K135" t="s" s="2">
+        <v>724</v>
+      </c>
+      <c r="L135" t="s" s="2">
         <v>725</v>
       </c>
-      <c r="L135" t="s" s="2">
+      <c r="M135" t="s" s="2">
         <v>726</v>
       </c>
-      <c r="M135" t="s" s="2">
+      <c r="N135" t="s" s="2">
+        <v>694</v>
+      </c>
+      <c r="O135" t="s" s="2">
         <v>727</v>
-      </c>
-      <c r="N135" t="s" s="2">
-        <v>695</v>
-      </c>
-      <c r="O135" t="s" s="2">
-        <v>728</v>
       </c>
       <c r="P135" t="s" s="2">
         <v>74</v>
@@ -17233,7 +17230,7 @@
         <v>74</v>
       </c>
       <c r="AF135" t="s" s="2">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="AG135" t="s" s="2">
         <v>75</v>
@@ -17248,7 +17245,7 @@
         <v>362</v>
       </c>
       <c r="AK135" t="s" s="2">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="AL135" t="s" s="2">
         <v>74</v>

</xml_diff>